<commit_message>
added data to data file
</commit_message>
<xml_diff>
--- a/Copy of data.xlsx
+++ b/Copy of data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asrat Mekonnen\Documents\New Project-Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53CC9549-4E29-4142-AD53-C3E5DFAAB262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F45D483-BA1F-4CF4-A991-7EA971B5CF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{42B01188-EA38-4BA5-BABB-021FB0FAFC58}"/>
   </bookViews>
@@ -379,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5311EA-DD38-4E4D-BA6C-1BC90B543383}">
-  <dimension ref="A1:A101"/>
+  <dimension ref="A1:A105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -892,6 +892,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>